<commit_message>
i want to shoot myself
</commit_message>
<xml_diff>
--- a/Grade10List.xlsx
+++ b/Grade10List.xlsx
@@ -3,26 +3,27 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yasharora/Desktop/School/CompSci/SignInSystem/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E4DFB65-382E-E148-9140-614A9115A4D4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{A0289CAB-6866-B84C-B66B-2E28F2BCF590}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="560" windowWidth="28040" windowHeight="17440" activeTab="5" xr2:uid="{5EAFCAD1-2523-D746-8D75-176EC8CBF95B}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{DE3DE74F-B9EB-844A-A379-0C0BC4B8336B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Master" sheetId="2" r:id="rId1"/>
-    <sheet name="Test" sheetId="3" r:id="rId2"/>
-    <sheet name="Chill Zone" sheetId="4" r:id="rId3"/>
-    <sheet name="Quiet Work" sheetId="5" r:id="rId4"/>
-    <sheet name="Academic Support" sheetId="6" r:id="rId5"/>
-    <sheet name="Group Work" sheetId="7" r:id="rId6"/>
+    <sheet name="Master" sheetId="1" r:id="rId1"/>
+    <sheet name="Test" sheetId="2" r:id="rId2"/>
+    <sheet name="Chill Zone" sheetId="3" r:id="rId3"/>
+    <sheet name="Quiet Work" sheetId="4" r:id="rId4"/>
+    <sheet name="Academic Support" sheetId="5" r:id="rId5"/>
+    <sheet name="Group Work" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="16">
   <si>
     <t>Student Number</t>
   </si>
@@ -57,12 +58,34 @@
   </si>
   <si>
     <t>Subject Missed</t>
+  </si>
+  <si>
+    <t>111111111</t>
+  </si>
+  <si>
+    <t>Yash</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Geography</t>
+  </si>
+  <si>
+    <t>Group Work</t>
+  </si>
+  <si>
+    <t>Music</t>
+  </si>
+  <si>
+    <t>Art</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -92,10 +115,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,19 +436,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB8261B4-E6AE-8A4D-B294-53E2B203ED59}">
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="4" max="4" width="11.6640625" customWidth="1" collapsed="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -450,10 +474,63 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D2" s="1"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="5" t="n">
+        <v>43426.89297035879</v>
+      </c>
+      <c r="E2" s="6" t="n">
+        <v>43426.89297035879</v>
+      </c>
+      <c r="F2" s="6" t="n">
+        <v>43426.893146863425</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="3">
+        <v>43426.891656747684</v>
+      </c>
+      <c r="E2" s="4">
+        <v>43426.891656747684</v>
+      </c>
+      <c r="F2" s="4">
+        <v>43426.891742974534</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -468,7 +545,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -504,6 +581,48 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -512,7 +631,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -545,48 +664,6 @@
       <c r="D2" s="1"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:I1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -601,7 +678,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -637,15 +714,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -672,6 +749,64 @@
       </c>
       <c r="I1" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="5" t="n">
+        <v>43426.89297035879</v>
+      </c>
+      <c r="E2" s="6" t="n">
+        <v>43426.89297035879</v>
+      </c>
+      <c r="F2" s="6" t="n">
+        <v>43426.893146863425</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="3">
+        <v>43426.891656747684</v>
+      </c>
+      <c r="E2" s="4">
+        <v>43426.891656747684</v>
+      </c>
+      <c r="F2" s="4">
+        <v>43426.891742974534</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>